<commit_message>
Ajustes na tabela de investimentos
</commit_message>
<xml_diff>
--- a/Trabalho 2/Experiments.xlsx
+++ b/Trabalho 2/Experiments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>N/A</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Crossover Percentage</t>
+  </si>
+  <si>
+    <t>[90%, 100%]:</t>
+  </si>
+  <si>
+    <t>[70%, 89%]:</t>
+  </si>
+  <si>
+    <t>[50%, 69%]:</t>
+  </si>
+  <si>
+    <t>&lt; 50%:</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -154,6 +166,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,8 +498,8 @@
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>0</v>
+      <c r="C3" s="9">
+        <v>1000</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
@@ -506,10 +521,10 @@
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="9">
         <v>100</v>
       </c>
       <c r="E4" s="7">
@@ -529,10 +544,10 @@
       <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="9">
         <v>100</v>
       </c>
       <c r="E5" s="7">
@@ -552,10 +567,10 @@
       <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="C6" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="9">
         <v>100</v>
       </c>
       <c r="E6" s="7">
@@ -699,10 +714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G130"/>
+  <dimension ref="B2:K130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G5"/>
+      <selection activeCell="B2" sqref="B2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -714,9 +729,10 @@
     <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -736,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <v>100</v>
       </c>
@@ -755,8 +771,14 @@
       <c r="G3" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>100</v>
       </c>
@@ -775,8 +797,14 @@
       <c r="G4" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>100</v>
       </c>
@@ -795,8 +823,14 @@
       <c r="G5" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>100</v>
       </c>
@@ -815,8 +849,14 @@
       <c r="G6" s="8">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>100</v>
       </c>
@@ -836,7 +876,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>100</v>
       </c>
@@ -856,7 +896,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>100</v>
       </c>
@@ -876,7 +916,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>100</v>
       </c>
@@ -896,7 +936,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>100</v>
       </c>
@@ -916,7 +956,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>100</v>
       </c>
@@ -936,7 +976,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>100</v>
       </c>
@@ -956,7 +996,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>100</v>
       </c>
@@ -976,7 +1016,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>100</v>
       </c>
@@ -996,7 +1036,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>10</v>
       </c>

</xml_diff>